<commit_message>
Created dataprovider to handle multiple set of data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DBTestData/QA_DB_TEST_DATA.xlsx
+++ b/src/test/resources/testData/DBTestData/QA_DB_TEST_DATA.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komal.Phadtare\MyWorkSpace\HybridFramework\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komal.Phadtare\MyWorkSpace\HybridFramework\src\test\resources\testData\DBTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB690E-D1DC-491C-A120-32A1C630F973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE5B95C-B237-4689-B5D9-249ED122BA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
     <sheet name="TC02" sheetId="2" r:id="rId2"/>
+    <sheet name="TC03" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>quertToGetCount</t>
   </si>
@@ -40,9 +41,6 @@
     <t>SELECT patient_id,age,email FROM sys.patients_data where first_name= "Amalee";</t>
   </si>
   <si>
-    <t>expectedID</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -56,13 +54,40 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>SELECT patient_id,first_name,age,email FROM sys.patients_data where first_name= "Donnie";</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>dmillwater3@aboutads.info</t>
+  </si>
+  <si>
+    <t>SELECT patient_id,first_name,age,email FROM sys.patients_data where first_name= "Rikki";</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>rtippertonl@addthis.com</t>
+  </si>
+  <si>
+    <t>patientID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +99,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,10 +133,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -388,7 +435,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,8 +443,8 @@
     <col min="1" max="1" width="35.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -413,49 +460,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE3B4ED-1C1D-4894-9289-4495E51397D9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="87.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{1AE31C0A-4676-4F83-B479-76C68D6034E7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{513C0D0D-FE3E-449F-9522-9860EBDC8455}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50BEA87-14FC-48DF-AEA8-ABC4E600B315}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="102.1796875" customWidth="1"/>
+    <col min="2" max="2" width="2.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{1336E1D3-1052-4094-B531-1BD11ED464E2}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{0689ADBD-22BA-4CFF-901B-14C4D6C0A67F}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{94306CC8-6B5F-4DE8-B91F-9A3282B05B06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
To compare Excel data with DB
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DBTestData/QA_DB_TEST_DATA.xlsx
+++ b/src/test/resources/testData/DBTestData/QA_DB_TEST_DATA.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komal.Phadtare\MyWorkSpace\HybridFramework\src\test\resources\testData\DBTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE5B95C-B237-4689-B5D9-249ED122BA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4C3683-C581-4707-A81B-8A7CD344352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
     <sheet name="TC02" sheetId="2" r:id="rId2"/>
     <sheet name="TC03" sheetId="4" r:id="rId3"/>
+    <sheet name="TC04" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>quertToGetCount</t>
   </si>
@@ -81,6 +82,90 @@
   </si>
   <si>
     <t>patientID</t>
+  </si>
+  <si>
+    <t>SELECT patient_id, first_name,age,email FROM sys.patients_data limit 10;</t>
+  </si>
+  <si>
+    <t>mlufkin0@prlog.org</t>
+  </si>
+  <si>
+    <t>Minna</t>
+  </si>
+  <si>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>acurr1@skyrock.com</t>
+  </si>
+  <si>
+    <t>Janel</t>
+  </si>
+  <si>
+    <t>jbourgourd2@prlog.org</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Donnie</t>
+  </si>
+  <si>
+    <t>Issi</t>
+  </si>
+  <si>
+    <t>iraggles4@globo.com</t>
+  </si>
+  <si>
+    <t>Vaclav</t>
+  </si>
+  <si>
+    <t>vdjakovic5@altervista.org</t>
+  </si>
+  <si>
+    <t>mbourdel6@e-recht24.de</t>
+  </si>
+  <si>
+    <t>Murray</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>daccomb7@people.com.cn</t>
+  </si>
+  <si>
+    <t>Marlena</t>
+  </si>
+  <si>
+    <t>mvanderson8@wikispaces.com</t>
+  </si>
+  <si>
+    <t>aegdell9@oaic.gov.au</t>
+  </si>
+  <si>
+    <t>Amalee</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>patientId</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>46</t>
   </si>
 </sst>
 </file>
@@ -120,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -128,12 +213,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -145,12 +245,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,7 +542,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,7 +570,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,17 +609,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -543,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50BEA87-14FC-48DF-AEA8-ABC4E600B315}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -568,16 +675,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -602,4 +709,207 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7778AA-7FCB-4804-946A-7B866133A3D2}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="62.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="12">
+        <v>73</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12">
+        <v>50</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="12">
+        <v>78</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="12">
+        <v>18</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="12">
+        <v>84</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="12">
+        <v>84</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="12">
+        <v>52</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{89D8AB8B-6DED-494B-8BFD-8923FB364EF9}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B2BF47CD-E221-4EC0-9BF0-14572A36704A}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FA4B5219-B8D8-4360-AE12-9B4BD8EB3845}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{147F7A05-FE22-4B8D-99A0-7E2CF23D98FE}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{F6A0A5C9-8079-42DB-AC81-52041F638774}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{0FDF6AB6-3152-4C8F-94C6-2C2936A87C16}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{12AF8149-C4D3-43A8-897F-AC7D08CAD177}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{619F3A13-A0D0-4B22-9AB4-4510D2DECCC9}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{3B5E4632-89B4-48D5-AF9F-8258051C3A46}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{DB09B818-038D-447E-9625-62AE92A444A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>